<commit_message>
updat today time and add time for next two days
</commit_message>
<xml_diff>
--- a/04.02-01.03.xlsx
+++ b/04.02-01.03.xlsx
@@ -49,6 +49,21 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
+с вычетом на английский</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Anna Sharuntsova.EX
 с вычетом на английский</t>
         </r>
       </text>
@@ -218,10 +233,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -512,7 +527,7 @@
   <dimension ref="B2:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F7"/>
+      <selection activeCell="M3" sqref="M3:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +561,7 @@
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1">
@@ -567,14 +582,22 @@
       <c r="H3" s="7">
         <v>8</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="7"/>
+      <c r="I3" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="J3" s="7">
+        <v>7</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="L3" s="7">
+        <v>8</v>
+      </c>
       <c r="M3" s="8"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="10"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="1">
         <v>0.82291666666666663</v>
       </c>
@@ -587,9 +610,13 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="H4" s="7"/>
-      <c r="I4" s="1"/>
+      <c r="I4" s="1">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="J4" s="7"/>
-      <c r="K4" s="1"/>
+      <c r="K4" s="1">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="L4" s="7"/>
       <c r="M4" s="8"/>
     </row>
@@ -600,17 +627,21 @@
       <c r="C6" s="1">
         <v>0.48958333333333331</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="10">
         <v>8</v>
       </c>
       <c r="E6" s="1">
         <v>0.4375</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <v>8</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="11"/>
+      <c r="G6" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="H6" s="10">
+        <v>6</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="9"/>
       <c r="K6" s="1"/>
@@ -622,13 +653,15 @@
       <c r="C7" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="11"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="H7" s="10"/>
       <c r="I7" s="1"/>
       <c r="J7" s="9"/>
       <c r="K7" s="1"/>
@@ -651,7 +684,7 @@
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="1"/>
@@ -667,7 +700,7 @@
       <c r="M11" s="8"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="1"/>
       <c r="D12" s="7"/>
       <c r="E12" s="1"/>
@@ -726,7 +759,7 @@
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="1"/>
@@ -742,7 +775,7 @@
       <c r="M19" s="8"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="1"/>
       <c r="D20" s="7"/>
       <c r="E20" s="1"/>
@@ -801,7 +834,7 @@
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C27" s="1"/>
@@ -817,7 +850,7 @@
       <c r="M27" s="8"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="1"/>
       <c r="D28" s="7"/>
       <c r="E28" s="1"/>
@@ -835,33 +868,75 @@
         <v>2</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="11"/>
+      <c r="D30" s="10"/>
       <c r="E30" s="1"/>
       <c r="F30" s="9"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="11"/>
+      <c r="H30" s="10"/>
       <c r="I30" s="1"/>
       <c r="J30" s="9"/>
       <c r="K30" s="1"/>
-      <c r="L30" s="11"/>
+      <c r="L30" s="10"/>
       <c r="M30" s="8"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="9"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="11"/>
+      <c r="D31" s="10"/>
       <c r="E31" s="1"/>
       <c r="F31" s="9"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="11"/>
+      <c r="H31" s="10"/>
       <c r="I31" s="1"/>
       <c r="J31" s="9"/>
       <c r="K31" s="1"/>
-      <c r="L31" s="11"/>
+      <c r="L31" s="10"/>
       <c r="M31" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="J11:J12"/>
     <mergeCell ref="J27:J28"/>
     <mergeCell ref="L27:L28"/>
     <mergeCell ref="M27:M28"/>
@@ -876,48 +951,6 @@
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="F27:F28"/>
     <mergeCell ref="H27:H28"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="J19:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fill intended time for week and update today actual time
</commit_message>
<xml_diff>
--- a/04.02-01.03.xlsx
+++ b/04.02-01.03.xlsx
@@ -289,10 +289,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
@@ -585,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19:D20"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +620,7 @@
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1">
@@ -656,7 +656,7 @@
       <c r="M3" s="8"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="11"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="1">
         <v>0.82291666666666663</v>
       </c>
@@ -686,19 +686,19 @@
       <c r="C6" s="1">
         <v>0.48958333333333331</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="11">
         <v>8</v>
       </c>
       <c r="E6" s="1">
         <v>0.4375</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="11">
         <v>8</v>
       </c>
       <c r="G6" s="1">
         <v>0.45833333333333331</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="11">
         <v>6</v>
       </c>
       <c r="I6" s="1">
@@ -722,15 +722,15 @@
       <c r="C7" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="F7" s="10"/>
+      <c r="F7" s="11"/>
       <c r="G7" s="1">
         <v>0.70833333333333337</v>
       </c>
-      <c r="H7" s="10"/>
+      <c r="H7" s="11"/>
       <c r="I7" s="1">
         <v>0.77777777777777779</v>
       </c>
@@ -757,7 +757,7 @@
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="1">
@@ -791,7 +791,7 @@
       <c r="M11" s="8"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="11"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="1">
         <v>0.82291666666666663</v>
       </c>
@@ -819,13 +819,13 @@
       <c r="C14" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="11">
         <v>6.5</v>
       </c>
       <c r="E14" s="1">
         <v>0.625</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14" s="11">
         <v>4</v>
       </c>
       <c r="G14" s="1">
@@ -855,11 +855,11 @@
       <c r="C15" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="F15" s="10"/>
+      <c r="F15" s="11"/>
       <c r="G15" s="1">
         <v>0.82291666666666663</v>
       </c>
@@ -890,7 +890,7 @@
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C19" s="1">
@@ -905,16 +905,28 @@
       <c r="F19" s="7">
         <v>4.5</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="7"/>
+      <c r="G19" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H19" s="7">
+        <v>7</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="J19" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L19" s="7">
+        <v>5</v>
+      </c>
       <c r="M19" s="8"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="11"/>
+      <c r="B20" s="10"/>
       <c r="C20" s="1">
         <v>0.75</v>
       </c>
@@ -923,11 +935,17 @@
         <v>0.8125</v>
       </c>
       <c r="F20" s="7"/>
-      <c r="G20" s="1"/>
+      <c r="G20" s="1">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="H20" s="7"/>
-      <c r="I20" s="1"/>
+      <c r="I20" s="1">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="J20" s="7"/>
-      <c r="K20" s="1"/>
+      <c r="K20" s="1">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="L20" s="7"/>
       <c r="M20" s="8"/>
     </row>
@@ -941,8 +959,12 @@
       <c r="D22" s="9">
         <v>4</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="9"/>
+      <c r="E22" s="1">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="F22" s="9">
+        <v>5.5</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="H22" s="9"/>
       <c r="I22" s="1"/>
@@ -957,7 +979,9 @@
         <v>0.75</v>
       </c>
       <c r="D23" s="9"/>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1">
+        <v>0.81944444444444453</v>
+      </c>
       <c r="F23" s="9"/>
       <c r="G23" s="1"/>
       <c r="H23" s="9"/>
@@ -983,7 +1007,7 @@
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C27" s="1"/>
@@ -999,7 +1023,7 @@
       <c r="M27" s="8"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="11"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="1"/>
       <c r="D28" s="7"/>
       <c r="E28" s="1"/>
@@ -1017,33 +1041,75 @@
         <v>2</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="10"/>
+      <c r="D30" s="11"/>
       <c r="E30" s="1"/>
       <c r="F30" s="9"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="10"/>
+      <c r="H30" s="11"/>
       <c r="I30" s="1"/>
       <c r="J30" s="9"/>
       <c r="K30" s="1"/>
-      <c r="L30" s="10"/>
+      <c r="L30" s="11"/>
       <c r="M30" s="8"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="9"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="10"/>
+      <c r="D31" s="11"/>
       <c r="E31" s="1"/>
       <c r="F31" s="9"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="10"/>
+      <c r="H31" s="11"/>
       <c r="I31" s="1"/>
       <c r="J31" s="9"/>
       <c r="K31" s="1"/>
-      <c r="L31" s="10"/>
+      <c r="L31" s="11"/>
       <c r="M31" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="M3:M4"/>
     <mergeCell ref="L19:L20"/>
     <mergeCell ref="M19:M20"/>
     <mergeCell ref="B22:B23"/>
@@ -1058,48 +1124,6 @@
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="J19:J20"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J27:J28"/>
-    <mergeCell ref="L27:L28"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="L30:L31"/>
-    <mergeCell ref="M30:M31"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="H27:H28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fill actual today time
</commit_message>
<xml_diff>
--- a/04.02-01.03.xlsx
+++ b/04.02-01.03.xlsx
@@ -642,7 +642,7 @@
   <dimension ref="B2:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30:J31"/>
+      <selection activeCell="M30" sqref="M30:M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,9 +1196,15 @@
       <c r="J30" s="9">
         <v>4.5</v>
       </c>
-      <c r="K30" s="1"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="8"/>
+      <c r="K30" s="1">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="L30" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="M30" s="8">
+        <v>25</v>
+      </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="9"/>
@@ -1216,7 +1222,9 @@
         <v>0.73611111111111116</v>
       </c>
       <c r="J31" s="9"/>
-      <c r="K31" s="1"/>
+      <c r="K31" s="1">
+        <v>0.75694444444444453</v>
+      </c>
       <c r="L31" s="11"/>
       <c r="M31" s="8"/>
     </row>

</xml_diff>